<commit_message>
udfyldt dagslog og tidsplan for dagens arbejde.
</commit_message>
<xml_diff>
--- a/Assets/Documents/Estimeret_tidsplan.xlsx
+++ b/Assets/Documents/Estimeret_tidsplan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\92agg\Desktop\Svendeprøve\Assets\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{434D603B-F224-4AD6-82BB-4100A0C56ACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D31A7E11-7DB8-4329-9A73-DCF882ED7C92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{221EF780-FBBD-4846-90E3-EFC5DE4BA05F}"/>
+    <workbookView xWindow="-16320" yWindow="-7260" windowWidth="16440" windowHeight="28320" xr2:uid="{221EF780-FBBD-4846-90E3-EFC5DE4BA05F}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -438,6 +438,36 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -446,36 +476,6 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -798,8 +798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C0E67C9-148C-445C-AEDA-6C5F365E02ED}">
   <dimension ref="B1:AB61"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T61" sqref="T61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -811,13 +811,13 @@
   <sheetData>
     <row r="1" spans="2:28" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:28" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -829,14 +829,14 @@
     </row>
     <row r="3" spans="2:28" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="29"/>
-      <c r="D4" s="30">
+      <c r="C4" s="39"/>
+      <c r="D4" s="40">
         <v>45391</v>
       </c>
-      <c r="E4" s="30"/>
+      <c r="E4" s="40"/>
     </row>
     <row r="5" spans="2:28" ht="11.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="2:28" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1026,17 +1026,17 @@
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
+      <c r="N11" s="19"/>
       <c r="O11" s="5"/>
       <c r="P11" s="5"/>
       <c r="Q11" s="5"/>
       <c r="R11" s="5"/>
-      <c r="S11" s="5"/>
+      <c r="S11" s="19"/>
       <c r="T11" s="5"/>
       <c r="U11" s="5"/>
       <c r="V11" s="5"/>
       <c r="W11" s="5"/>
-      <c r="X11" s="5"/>
+      <c r="X11" s="19"/>
       <c r="Z11" s="20"/>
       <c r="AB11" s="4" t="s">
         <v>26</v>
@@ -1074,56 +1074,56 @@
       <c r="B13" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="31"/>
-      <c r="I13" s="31"/>
-      <c r="J13" s="31"/>
-      <c r="K13" s="31"/>
-      <c r="L13" s="31"/>
-      <c r="M13" s="31"/>
-      <c r="N13" s="31"/>
-      <c r="O13" s="31"/>
-      <c r="P13" s="31"/>
-      <c r="Q13" s="31"/>
-      <c r="R13" s="31"/>
-      <c r="S13" s="31"/>
-      <c r="T13" s="31"/>
-      <c r="U13" s="31"/>
-      <c r="V13" s="31"/>
-      <c r="W13" s="31"/>
-      <c r="X13" s="39"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="28"/>
+      <c r="N13" s="28"/>
+      <c r="O13" s="28"/>
+      <c r="P13" s="28"/>
+      <c r="Q13" s="28"/>
+      <c r="R13" s="28"/>
+      <c r="S13" s="28"/>
+      <c r="T13" s="28"/>
+      <c r="U13" s="28"/>
+      <c r="V13" s="28"/>
+      <c r="W13" s="28"/>
+      <c r="X13" s="36"/>
       <c r="Z13" s="9"/>
       <c r="AB13" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="2:28" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="34" t="s">
+      <c r="B14" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="35"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
-      <c r="J14" s="35"/>
-      <c r="K14" s="35"/>
-      <c r="L14" s="35"/>
-      <c r="M14" s="35"/>
-      <c r="N14" s="35"/>
-      <c r="O14" s="35"/>
-      <c r="P14" s="35"/>
-      <c r="Q14" s="35"/>
-      <c r="R14" s="35"/>
-      <c r="S14" s="35"/>
-      <c r="T14" s="35"/>
-      <c r="U14" s="35"/>
-      <c r="V14" s="35"/>
-      <c r="W14" s="35"/>
-      <c r="X14" s="36"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="32"/>
+      <c r="L14" s="32"/>
+      <c r="M14" s="32"/>
+      <c r="N14" s="32"/>
+      <c r="O14" s="32"/>
+      <c r="P14" s="32"/>
+      <c r="Q14" s="32"/>
+      <c r="R14" s="32"/>
+      <c r="S14" s="32"/>
+      <c r="T14" s="32"/>
+      <c r="U14" s="32"/>
+      <c r="V14" s="32"/>
+      <c r="W14" s="32"/>
+      <c r="X14" s="33"/>
       <c r="Z14" s="21"/>
       <c r="AB14" s="4" t="s">
         <v>6</v>
@@ -1135,7 +1135,7 @@
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
-      <c r="H15" s="40"/>
+      <c r="H15" s="37"/>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
@@ -1309,52 +1309,52 @@
       <c r="B22" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F22" s="31"/>
-      <c r="G22" s="31"/>
-      <c r="H22" s="31"/>
-      <c r="I22" s="31"/>
-      <c r="J22" s="31"/>
-      <c r="K22" s="31"/>
-      <c r="L22" s="31"/>
-      <c r="M22" s="31"/>
-      <c r="N22" s="31"/>
-      <c r="O22" s="31"/>
-      <c r="P22" s="37"/>
-      <c r="Q22" s="31"/>
-      <c r="R22" s="31"/>
-      <c r="S22" s="31"/>
-      <c r="T22" s="31"/>
-      <c r="U22" s="31"/>
-      <c r="V22" s="31"/>
-      <c r="W22" s="31"/>
-      <c r="X22" s="31"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="28"/>
+      <c r="I22" s="28"/>
+      <c r="J22" s="28"/>
+      <c r="K22" s="28"/>
+      <c r="L22" s="28"/>
+      <c r="M22" s="28"/>
+      <c r="N22" s="28"/>
+      <c r="O22" s="28"/>
+      <c r="P22" s="34"/>
+      <c r="Q22" s="28"/>
+      <c r="R22" s="28"/>
+      <c r="S22" s="28"/>
+      <c r="T22" s="28"/>
+      <c r="U22" s="28"/>
+      <c r="V22" s="28"/>
+      <c r="W22" s="28"/>
+      <c r="X22" s="28"/>
     </row>
     <row r="23" spans="2:24" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="34" t="s">
+      <c r="B23" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="35"/>
-      <c r="F23" s="35"/>
-      <c r="G23" s="35"/>
-      <c r="H23" s="35"/>
-      <c r="I23" s="35"/>
-      <c r="J23" s="35"/>
-      <c r="K23" s="35"/>
-      <c r="L23" s="35"/>
-      <c r="M23" s="35"/>
-      <c r="N23" s="35"/>
-      <c r="O23" s="35"/>
-      <c r="P23" s="35"/>
-      <c r="Q23" s="35"/>
-      <c r="R23" s="35"/>
-      <c r="S23" s="35"/>
-      <c r="T23" s="35"/>
-      <c r="U23" s="35"/>
-      <c r="V23" s="35"/>
-      <c r="W23" s="35"/>
-      <c r="X23" s="36"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="32"/>
+      <c r="I23" s="32"/>
+      <c r="J23" s="32"/>
+      <c r="K23" s="32"/>
+      <c r="L23" s="32"/>
+      <c r="M23" s="32"/>
+      <c r="N23" s="32"/>
+      <c r="O23" s="32"/>
+      <c r="P23" s="32"/>
+      <c r="Q23" s="32"/>
+      <c r="R23" s="32"/>
+      <c r="S23" s="32"/>
+      <c r="T23" s="32"/>
+      <c r="U23" s="32"/>
+      <c r="V23" s="32"/>
+      <c r="W23" s="32"/>
+      <c r="X23" s="33"/>
     </row>
     <row r="24" spans="2:24" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
@@ -1362,8 +1362,8 @@
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="38"/>
+      <c r="H24" s="35"/>
+      <c r="I24" s="35"/>
       <c r="J24" s="7"/>
       <c r="K24" s="7"/>
       <c r="L24" s="7"/>
@@ -1432,52 +1432,52 @@
       <c r="B27" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="32"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
-      <c r="K27" s="31"/>
-      <c r="L27" s="31"/>
-      <c r="M27" s="31"/>
-      <c r="N27" s="31"/>
-      <c r="O27" s="31"/>
-      <c r="P27" s="31"/>
-      <c r="Q27" s="31"/>
-      <c r="R27" s="31"/>
-      <c r="S27" s="31"/>
-      <c r="T27" s="31"/>
-      <c r="U27" s="31"/>
-      <c r="V27" s="31"/>
-      <c r="W27" s="31"/>
-      <c r="X27" s="31"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="28"/>
+      <c r="J27" s="28"/>
+      <c r="K27" s="28"/>
+      <c r="L27" s="28"/>
+      <c r="M27" s="28"/>
+      <c r="N27" s="28"/>
+      <c r="O27" s="28"/>
+      <c r="P27" s="28"/>
+      <c r="Q27" s="28"/>
+      <c r="R27" s="28"/>
+      <c r="S27" s="28"/>
+      <c r="T27" s="28"/>
+      <c r="U27" s="28"/>
+      <c r="V27" s="28"/>
+      <c r="W27" s="28"/>
+      <c r="X27" s="28"/>
     </row>
     <row r="28" spans="2:24" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="34" t="s">
+      <c r="B28" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="35"/>
-      <c r="D28" s="35"/>
-      <c r="E28" s="35"/>
-      <c r="F28" s="35"/>
-      <c r="G28" s="35"/>
-      <c r="H28" s="35"/>
-      <c r="I28" s="35"/>
-      <c r="J28" s="35"/>
-      <c r="K28" s="35"/>
-      <c r="L28" s="35"/>
-      <c r="M28" s="35"/>
-      <c r="N28" s="35"/>
-      <c r="O28" s="35"/>
-      <c r="P28" s="35"/>
-      <c r="Q28" s="35"/>
-      <c r="R28" s="35"/>
-      <c r="S28" s="35"/>
-      <c r="T28" s="35"/>
-      <c r="U28" s="35"/>
-      <c r="V28" s="35"/>
-      <c r="W28" s="35"/>
-      <c r="X28" s="36"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
+      <c r="K28" s="32"/>
+      <c r="L28" s="32"/>
+      <c r="M28" s="32"/>
+      <c r="N28" s="32"/>
+      <c r="O28" s="32"/>
+      <c r="P28" s="32"/>
+      <c r="Q28" s="32"/>
+      <c r="R28" s="32"/>
+      <c r="S28" s="32"/>
+      <c r="T28" s="32"/>
+      <c r="U28" s="32"/>
+      <c r="V28" s="32"/>
+      <c r="W28" s="32"/>
+      <c r="X28" s="33"/>
     </row>
     <row r="29" spans="2:24" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
@@ -1485,7 +1485,7 @@
       </c>
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
-      <c r="H29" s="33"/>
+      <c r="H29" s="30"/>
       <c r="I29" s="7"/>
       <c r="J29" s="7"/>
       <c r="K29" s="7"/>

</xml_diff>